<commit_message>
Fix multi-year CDCM models and various minor improvements.
</commit_message>
<xml_diff>
--- a/models/Metadata.xlsx
+++ b/models/Metadata.xlsx
@@ -529,9 +529,6 @@
     <t>SSEN SHEPD</t>
   </si>
   <si>
-    <t>Dragon</t>
-  </si>
-  <si>
     <t>Utility Distribution Networks (not yet active)</t>
   </si>
   <si>
@@ -542,6 +539,9 @@
   </si>
   <si>
     <t>Short name</t>
+  </si>
+  <si>
+    <t>UDN</t>
   </si>
 </sst>
 </file>
@@ -614,8 +614,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="197">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -845,7 +847,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="197">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -944,6 +946,7 @@
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1042,6 +1045,7 @@
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1406,7 +1410,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1430,7 +1434,7 @@
         <v>163</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>157</v>
@@ -2220,10 +2224,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
@@ -2233,7 +2237,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L24" s="11">
         <v>10068882</v>
@@ -2267,7 +2271,7 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>

</xml_diff>

<commit_message>
Metadata update (information on newer and prospective IDNOs).
</commit_message>
<xml_diff>
--- a/models/Metadata.xlsx
+++ b/models/Metadata.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="320" windowWidth="28000" windowHeight="13240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28480" windowHeight="14580" tabRatio="393"/>
   </bookViews>
   <sheets>
     <sheet name="Distributors and GSP Groups" sheetId="1" r:id="rId1"/>
     <sheet name="Measurement Classes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Distributors and GSP Groups'!$A$1:$L$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Distributors and GSP Groups'!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="186">
   <si>
     <t>WPD EastM</t>
   </si>
@@ -493,9 +493,6 @@
     <t>J1310 identifier</t>
   </si>
   <si>
-    <t>J0002 identifier</t>
-  </si>
-  <si>
     <t>Ofgem 2014 identifier</t>
   </si>
   <si>
@@ -548,6 +545,42 @@
   </si>
   <si>
     <t>UDNL</t>
+  </si>
+  <si>
+    <t>EAPN</t>
+  </si>
+  <si>
+    <t>Energy Assets Power Networks</t>
+  </si>
+  <si>
+    <t>Energy Assets Power Networks Limited</t>
+  </si>
+  <si>
+    <t>Power On Connections</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Associated ICP</t>
+  </si>
+  <si>
+    <t>g2 Energy</t>
+  </si>
+  <si>
+    <t>Dragon Infrastructure</t>
+  </si>
+  <si>
+    <t>Harlaxton Engineering Services</t>
+  </si>
+  <si>
+    <t>BSC identifier</t>
+  </si>
+  <si>
+    <t>Energy Assets</t>
+  </si>
+  <si>
+    <t>EDFI</t>
   </si>
 </sst>
 </file>
@@ -620,7 +653,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -830,8 +863,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -862,8 +921,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -968,6 +1033,19 @@
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1072,6 +1150,19 @@
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1430,13 +1521,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1448,19 +1539,20 @@
     <col min="5" max="5" width="27.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" style="13" customWidth="1"/>
     <col min="11" max="11" width="40.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.83203125" style="3"/>
+    <col min="13" max="13" width="31.6640625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="42">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="42">
       <c r="A1" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>154</v>
@@ -1472,19 +1564,19 @@
         <v>131</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>155</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>125</v>
@@ -1492,8 +1584,11 @@
       <c r="L1" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1518,10 +1613,10 @@
       <c r="H2" s="2">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="12" t="s">
         <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
@@ -1530,8 +1625,9 @@
       <c r="L2" s="11">
         <v>2366949</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1556,10 +1652,10 @@
       <c r="H3" s="2">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="12" t="s">
         <v>36</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1568,8 +1664,9 @@
       <c r="L3" s="11">
         <v>2906953</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1594,10 +1691,10 @@
       <c r="H4" s="2">
         <v>23</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="12" t="s">
         <v>102</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -1606,8 +1703,9 @@
       <c r="L4" s="11">
         <v>4112320</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1632,10 +1730,10 @@
       <c r="H5" s="2">
         <v>18</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="12" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1644,8 +1742,9 @@
       <c r="L5" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1670,10 +1769,10 @@
       <c r="H6" s="2">
         <v>13</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="12" t="s">
         <v>28</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1682,16 +1781,17 @@
       <c r="L6" s="11">
         <v>2366937</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>67</v>
@@ -1708,10 +1808,10 @@
       <c r="H7" s="2">
         <v>20</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="12" t="s">
         <v>71</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1720,16 +1820,17 @@
       <c r="L7" s="11">
         <v>4094290</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>45</v>
@@ -1746,10 +1847,10 @@
       <c r="H8" s="2">
         <v>17</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="12" t="s">
         <v>48</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1758,8 +1859,9 @@
       <c r="L8" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1784,10 +1886,10 @@
       <c r="H9" s="2">
         <v>10</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1796,8 +1898,9 @@
       <c r="L9" s="11">
         <v>2366906</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1822,10 +1925,10 @@
       <c r="H10" s="2">
         <v>12</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1834,8 +1937,9 @@
       <c r="L10" s="11">
         <v>3929195</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1860,10 +1964,10 @@
       <c r="H11" s="2">
         <v>19</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="12" t="s">
         <v>57</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1872,8 +1976,9 @@
       <c r="L11" s="11">
         <v>3043097</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1898,10 +2003,10 @@
       <c r="H12" s="2">
         <v>11</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -1910,8 +2015,9 @@
       <c r="L12" s="11">
         <v>2366923</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1936,10 +2042,10 @@
       <c r="H13" s="2">
         <v>21</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="12" t="s">
         <v>87</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -1948,8 +2054,9 @@
       <c r="L13" s="11">
         <v>2366985</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1974,10 +2081,10 @@
       <c r="H14" s="2">
         <v>22</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="12" t="s">
         <v>65</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -1986,8 +2093,9 @@
       <c r="L14" s="11">
         <v>2366894</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2012,10 +2120,10 @@
       <c r="H15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="12" t="s">
         <v>95</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -2024,8 +2132,9 @@
       <c r="L15" s="11">
         <v>3600574</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2042,18 +2151,21 @@
       <c r="H16" s="2">
         <v>24</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="12"/>
       <c r="K16" s="1" t="s">
         <v>119</v>
       </c>
       <c r="L16" s="11">
         <v>4935008</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2070,18 +2182,19 @@
       <c r="H17" s="2">
         <v>25</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="1" t="s">
         <v>111</v>
       </c>
       <c r="L17" s="11">
         <v>4718806</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2098,18 +2211,21 @@
       <c r="H18" s="2">
         <v>26</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="1" t="s">
         <v>106</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2126,18 +2242,21 @@
       <c r="H19" s="2">
         <v>27</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="1" t="s">
         <v>115</v>
       </c>
       <c r="L19" s="11">
         <v>5581824</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2154,18 +2273,21 @@
       <c r="H20" s="2">
         <v>29</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="1" t="s">
         <v>122</v>
       </c>
       <c r="L20" s="11">
         <v>7330883</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2182,18 +2304,19 @@
       <c r="H21" s="2">
         <v>30</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="1" t="s">
         <v>128</v>
       </c>
       <c r="L21" s="11">
         <v>6684589</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2210,18 +2333,21 @@
       <c r="H22" s="2">
         <v>31</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="1" t="s">
         <v>134</v>
       </c>
       <c r="L22" s="11">
         <v>6339585</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2229,105 +2355,138 @@
         <v>136</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J23" s="1"/>
+      <c r="I23" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J23" s="12"/>
       <c r="K23" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L23" s="11">
         <v>9633506</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J24" s="1"/>
+      <c r="I24" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="J24" s="12"/>
       <c r="K24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L24" s="11">
         <v>10068882</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="2">
-        <v>88</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
       <c r="G25" s="1"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="1" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="L25" s="11">
-        <v>7255054</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>10326097</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="2">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="2">
+      <c r="H26" s="2"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L26" s="11">
+        <v>7255054</v>
+      </c>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="2">
+        <v>99</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="2">
         <v>28</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1" t="s">
+      <c r="I27" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L27" s="11">
         <v>6489447</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="L27" s="3"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="L28" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L26">
-    <sortState ref="A2:L26">
-      <sortCondition ref="A1:A26"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M27"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>